<commit_message>
PROS-7545 SANOFIAU Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/SANOFIAU/Data/Template.xlsx
+++ b/Projects/SANOFIAU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,24 +17,26 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$1:$G$97</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$1:$G$97</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$1:$G$97</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$1:$G$97</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$1:$G$97</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$1:$G$97</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Primary_Brand_Blocking!$A$2:$H$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$104</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$I$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2025,17 +2027,17 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
@@ -2294,17 +2296,17 @@
   </sheetPr>
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J92" activeCellId="0" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="66.1983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="12" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="5.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="11" width="9.10526315789474"/>
@@ -4460,10 +4462,10 @@
         <v>1</v>
       </c>
       <c r="H75" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4579,7 +4581,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,10 +4665,10 @@
         <v>1</v>
       </c>
       <c r="H82" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4840,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="I88" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4956,7 +4958,7 @@
         <v>1</v>
       </c>
       <c r="I92" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,7 +5074,7 @@
         <v>1</v>
       </c>
       <c r="I96" s="27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5128,19 +5130,19 @@
   </sheetPr>
   <dimension ref="1:94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="58.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="41" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="41" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="59.2348178137652"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="41" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="41" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="42" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="42" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="42" width="16.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="42" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -15996,17 +15998,17 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="60" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="60" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="60" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="60" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="60" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="60" width="5.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="60" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="61" width="5.1417004048583"/>
@@ -16252,7 +16254,7 @@
   </sheetPr>
   <dimension ref="1:62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -16260,13 +16262,13 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="82" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="82" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="82" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="82" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="82" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="82" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="82" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="82" width="67.2712550607288"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="82" width="5.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="82" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="83" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="83" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="83" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="83" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="83" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -17427,6 +17429,13 @@
       <c r="I11" s="88"/>
     </row>
     <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
       <c r="H12" s="88"/>
       <c r="I12" s="88"/>
       <c r="J12" s="0"/>
@@ -18446,6 +18455,13 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
       <c r="H13" s="88"/>
       <c r="I13" s="88"/>
       <c r="J13" s="0"/>
@@ -19465,6 +19481,13 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
       <c r="H14" s="88"/>
       <c r="I14" s="88"/>
       <c r="J14" s="0"/>
@@ -20484,6 +20507,13 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
       <c r="H15" s="88"/>
       <c r="I15" s="88"/>
       <c r="J15" s="0"/>
@@ -21503,6 +21533,13 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
       <c r="H16" s="88"/>
       <c r="I16" s="88"/>
       <c r="J16" s="0"/>
@@ -22522,6 +22559,13 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
       <c r="H17" s="88"/>
       <c r="I17" s="88"/>
       <c r="J17" s="0"/>
@@ -23541,6 +23585,13 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
       <c r="H18" s="88"/>
       <c r="I18" s="88"/>
       <c r="J18" s="0"/>
@@ -24560,6 +24611,13 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
       <c r="H19" s="88"/>
       <c r="I19" s="88"/>
       <c r="J19" s="0"/>
@@ -25579,6 +25637,13 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
       <c r="H20" s="88"/>
       <c r="I20" s="88"/>
       <c r="J20" s="0"/>
@@ -26598,6 +26663,13 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
       <c r="H21" s="88"/>
       <c r="I21" s="88"/>
       <c r="J21" s="0"/>
@@ -27617,6 +27689,13 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
       <c r="H22" s="88"/>
       <c r="I22" s="88"/>
       <c r="J22" s="0"/>
@@ -28636,6 +28715,13 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
       <c r="H23" s="88"/>
       <c r="I23" s="88"/>
       <c r="J23" s="0"/>
@@ -29655,6 +29741,13 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
       <c r="H24" s="88"/>
       <c r="I24" s="88"/>
       <c r="J24" s="0"/>
@@ -30674,6 +30767,13 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
       <c r="H25" s="88"/>
       <c r="I25" s="88"/>
       <c r="J25" s="0"/>
@@ -31726,6 +31826,13 @@
       <c r="I28" s="88"/>
     </row>
     <row r="29" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
       <c r="H29" s="88"/>
       <c r="I29" s="88"/>
       <c r="J29" s="0"/>
@@ -32745,6 +32852,13 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
       <c r="H30" s="88"/>
       <c r="I30" s="88"/>
       <c r="J30" s="0"/>
@@ -33924,21 +34038,21 @@
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="60" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="60" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="60" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="60" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="60" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="60" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="60" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="60" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="60" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="60" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="61" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="61" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="61" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="61" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -34065,7 +34179,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="97" t="n">
         <v>0</v>
@@ -34239,10 +34353,10 @@
         <v>2</v>
       </c>
       <c r="H11" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34268,10 +34382,10 @@
         <v>2</v>
       </c>
       <c r="H12" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34326,10 +34440,10 @@
         <v>2</v>
       </c>
       <c r="H14" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34442,10 +34556,10 @@
         <v>2</v>
       </c>
       <c r="H18" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34471,10 +34585,10 @@
         <v>2</v>
       </c>
       <c r="H19" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35138,10 +35252,10 @@
         <v>2</v>
       </c>
       <c r="H42" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35167,10 +35281,10 @@
         <v>2</v>
       </c>
       <c r="H43" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35196,7 +35310,7 @@
         <v>2</v>
       </c>
       <c r="H44" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="97" t="n">
         <v>0</v>
@@ -35312,10 +35426,10 @@
         <v>2</v>
       </c>
       <c r="H48" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35341,10 +35455,10 @@
         <v>2</v>
       </c>
       <c r="H49" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35370,10 +35484,10 @@
         <v>2</v>
       </c>
       <c r="H50" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35399,10 +35513,10 @@
         <v>2</v>
       </c>
       <c r="H51" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I51" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35428,10 +35542,10 @@
         <v>2</v>
       </c>
       <c r="H52" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35573,10 +35687,10 @@
         <v>2</v>
       </c>
       <c r="H57" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35747,10 +35861,10 @@
         <v>2</v>
       </c>
       <c r="H63" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35776,10 +35890,10 @@
         <v>2</v>
       </c>
       <c r="H64" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I64" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35805,10 +35919,10 @@
         <v>2</v>
       </c>
       <c r="H65" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35834,10 +35948,10 @@
         <v>2</v>
       </c>
       <c r="H66" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I66" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35950,10 +36064,10 @@
         <v>2</v>
       </c>
       <c r="H70" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I70" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35979,10 +36093,10 @@
         <v>2</v>
       </c>
       <c r="H71" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36008,10 +36122,10 @@
         <v>2</v>
       </c>
       <c r="H72" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I72" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36153,10 +36267,10 @@
         <v>2</v>
       </c>
       <c r="H77" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36298,10 +36412,10 @@
         <v>1</v>
       </c>
       <c r="H82" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36327,10 +36441,10 @@
         <v>2</v>
       </c>
       <c r="H83" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I83" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36356,10 +36470,10 @@
         <v>2</v>
       </c>
       <c r="H84" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I84" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36414,10 +36528,10 @@
         <v>2</v>
       </c>
       <c r="H86" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86" s="97" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36443,10 +36557,10 @@
         <v>2</v>
       </c>
       <c r="H87" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I87" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36472,10 +36586,10 @@
         <v>2</v>
       </c>
       <c r="H88" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I88" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36501,10 +36615,10 @@
         <v>1</v>
       </c>
       <c r="H89" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36617,10 +36731,10 @@
         <v>2</v>
       </c>
       <c r="H93" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I93" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36646,10 +36760,10 @@
         <v>2</v>
       </c>
       <c r="H94" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I94" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36675,10 +36789,10 @@
         <v>2</v>
       </c>
       <c r="H95" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I95" s="97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36736,7 +36850,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36943,7 +37057,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I102"/>
+  <autoFilter ref="A2:I104"/>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>

</xml_diff>